<commit_message>
final update to raw and processes data
</commit_message>
<xml_diff>
--- a/data/marburg/raw/marburg_parameter_new.xlsx
+++ b/data/marburg/raw/marburg_parameter_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/kem22_ic_ac_uk/Documents/Projects/Priority Pathogens/priority-pathogens/data/marburg/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cm401/priority_pathogen_review/data/marburg/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_BEA61AB98415BDB56D2A21CABEB3885871D94936" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{026625AA-AD92-42F4-9B6F-E92A94F7E193}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091C5CDF-D673-CB48-B6DE-13BB63956312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36945" yWindow="555" windowWidth="20715" windowHeight="14610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter_data___Table" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="222">
   <si>
     <t>Parameter_data_ID</t>
   </si>
@@ -485,9 +485,6 @@
   </si>
   <si>
     <t>Doubling time</t>
-  </si>
-  <si>
-    <t>2.0</t>
   </si>
   <si>
     <t>Human delay - serial interval</t>
@@ -1108,14 +1105,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AO12" sqref="AO12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="94.1640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="86.83203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="23.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1267,7 +1316,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1320,7 +1369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:50" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:50" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1331,16 +1380,16 @@
         <v>50</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>51</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="N3" s="1">
         <v>2</v>
@@ -1349,19 +1398,19 @@
         <v>186</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="T3" s="1" t="b">
         <v>0</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="W3" s="1" t="b">
         <v>0</v>
@@ -1373,10 +1422,10 @@
         <v>58</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AB3" s="1" t="b">
         <v>0</v>
@@ -1385,22 +1434,22 @@
         <v>0</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AG3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AH3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AI3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AJ3" s="2" t="s">
         <v>59</v>
@@ -1412,34 +1461,34 @@
         <v>65</v>
       </c>
       <c r="AP3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AQ3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AR3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AS3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AT3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AU3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AV3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AW3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AX3" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:50" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:50" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1450,16 +1499,16 @@
         <v>50</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>51</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="N4" s="1">
         <v>3</v>
@@ -1468,19 +1517,19 @@
         <v>100</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="T4" s="1" t="b">
         <v>0</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="W4" s="1" t="b">
         <v>0</v>
@@ -1492,10 +1541,10 @@
         <v>58</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AB4" s="1" t="b">
         <v>0</v>
@@ -1504,22 +1553,22 @@
         <v>0</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AF4" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AG4" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AH4" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AI4" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AJ4" s="2" t="s">
         <v>55</v>
@@ -1531,34 +1580,34 @@
         <v>65</v>
       </c>
       <c r="AP4" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AQ4" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AR4" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AS4" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AT4" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AU4" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AV4" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AW4" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AX4" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:50" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:50" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1570,16 +1619,16 @@
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>51</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="N5" s="1">
         <v>0</v>
@@ -1588,19 +1637,19 @@
         <v>224</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="T5" s="1" t="b">
         <v>0</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="W5" s="1" t="b">
         <v>0</v>
@@ -1612,10 +1661,10 @@
         <v>58</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AA5" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AB5" s="1" t="b">
         <v>0</v>
@@ -1624,22 +1673,22 @@
         <v>0</v>
       </c>
       <c r="AD5" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AG5" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AH5" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AI5" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AJ5" s="2" t="s">
         <v>59</v>
@@ -1651,34 +1700,34 @@
         <v>65</v>
       </c>
       <c r="AP5" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AQ5" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AR5" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AS5" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AT5" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AU5" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AV5" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AW5" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AX5" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:50" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:50" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -1689,16 +1738,16 @@
         <v>50</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>51</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="N6" s="1">
         <v>0</v>
@@ -1707,19 +1756,19 @@
         <v>63</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="T6" s="1" t="b">
         <v>0</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="W6" s="1" t="b">
         <v>0</v>
@@ -1731,10 +1780,10 @@
         <v>58</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AA6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AB6" s="1" t="b">
         <v>0</v>
@@ -1743,22 +1792,22 @@
         <v>0</v>
       </c>
       <c r="AD6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AE6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AF6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AG6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AH6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AI6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AJ6" s="2" t="s">
         <v>64</v>
@@ -1770,34 +1819,34 @@
         <v>65</v>
       </c>
       <c r="AP6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AQ6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AR6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AS6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AT6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AU6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AV6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AW6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AX6" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:50" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:50" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -1808,16 +1857,16 @@
         <v>50</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>51</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="N7" s="1">
         <v>0</v>
@@ -1826,19 +1875,19 @@
         <v>79</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="T7" s="1" t="b">
         <v>0</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="W7" s="1" t="b">
         <v>0</v>
@@ -1850,10 +1899,10 @@
         <v>58</v>
       </c>
       <c r="Z7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AA7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AB7" s="1" t="b">
         <v>0</v>
@@ -1862,22 +1911,22 @@
         <v>0</v>
       </c>
       <c r="AD7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AE7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AF7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AG7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AH7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AI7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AJ7" s="2" t="s">
         <v>64</v>
@@ -1889,34 +1938,34 @@
         <v>65</v>
       </c>
       <c r="AP7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AQ7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AR7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AS7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AT7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AU7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AV7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AW7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AX7" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>8</v>
       </c>
@@ -1966,7 +2015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>9</v>
       </c>
@@ -2022,7 +2071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>11</v>
       </c>
@@ -2084,7 +2133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>12</v>
       </c>
@@ -2149,7 +2198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>13</v>
       </c>
@@ -2199,7 +2248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>14</v>
       </c>
@@ -2264,7 +2313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>15</v>
       </c>
@@ -2314,7 +2363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>16</v>
       </c>
@@ -2376,7 +2425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>17</v>
       </c>
@@ -2441,7 +2490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>18</v>
       </c>
@@ -2494,7 +2543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>19</v>
       </c>
@@ -2580,7 +2629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>20</v>
       </c>
@@ -2639,7 +2688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>21</v>
       </c>
@@ -2710,7 +2759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>22</v>
       </c>
@@ -2772,7 +2821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>23</v>
       </c>
@@ -2831,7 +2880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>24</v>
       </c>
@@ -2899,7 +2948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>25</v>
       </c>
@@ -2970,7 +3019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>26</v>
       </c>
@@ -3044,7 +3093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>27</v>
       </c>
@@ -3100,7 +3149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>29</v>
       </c>
@@ -3150,7 +3199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>30</v>
       </c>
@@ -3206,7 +3255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>31</v>
       </c>
@@ -3232,7 +3281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>32</v>
       </c>
@@ -3303,7 +3352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>33</v>
       </c>
@@ -3365,7 +3414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>34</v>
       </c>
@@ -3415,7 +3464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>35</v>
       </c>
@@ -3474,7 +3523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>36</v>
       </c>
@@ -3542,7 +3591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>37</v>
       </c>
@@ -3622,7 +3671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>38</v>
       </c>
@@ -3669,7 +3718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>40</v>
       </c>
@@ -3755,7 +3804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>41</v>
       </c>
@@ -3841,7 +3890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>42</v>
       </c>
@@ -3927,7 +3976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>43</v>
       </c>
@@ -3983,7 +4032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>44</v>
       </c>
@@ -4069,7 +4118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>45</v>
       </c>
@@ -4155,7 +4204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>46</v>
       </c>
@@ -4241,7 +4290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>47</v>
       </c>
@@ -4294,7 +4343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>48</v>
       </c>
@@ -4380,7 +4429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>49</v>
       </c>
@@ -4421,7 +4470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>50</v>
       </c>
@@ -4429,7 +4478,10 @@
         <v>33</v>
       </c>
       <c r="C47" t="s">
-        <v>154</v>
+        <v>195</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
       </c>
       <c r="E47" t="s">
         <v>147</v>
@@ -4465,7 +4517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>51</v>
       </c>
@@ -4473,7 +4525,7 @@
         <v>31</v>
       </c>
       <c r="C48" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D48">
         <v>11</v>
@@ -4491,7 +4543,7 @@
         <v>15</v>
       </c>
       <c r="M48" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S48" t="b">
         <v>0</v>
@@ -4512,7 +4564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>52</v>
       </c>
@@ -4520,7 +4572,7 @@
         <v>27</v>
       </c>
       <c r="C49" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D49">
         <v>1.59</v>
@@ -4553,7 +4605,7 @@
         <v>82</v>
       </c>
       <c r="Z49" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AB49" t="b">
         <v>0</v>
@@ -4601,7 +4653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>53</v>
       </c>
@@ -4696,7 +4748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>54</v>
       </c>
@@ -4704,7 +4756,7 @@
         <v>35</v>
       </c>
       <c r="C51" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="S51" t="b">
         <v>0</v>
@@ -4722,22 +4774,22 @@
         <v>0</v>
       </c>
       <c r="AD51" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE51" t="s">
         <v>159</v>
       </c>
-      <c r="AE51" t="s">
+      <c r="AG51" t="s">
         <v>160</v>
       </c>
-      <c r="AG51" t="s">
+      <c r="AH51" t="s">
         <v>161</v>
       </c>
-      <c r="AH51" t="s">
-        <v>162</v>
-      </c>
       <c r="AX51" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>55</v>
       </c>
@@ -4784,7 +4836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>57</v>
       </c>
@@ -4843,19 +4895,19 @@
         <v>92</v>
       </c>
       <c r="AS53" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AU53" t="s">
         <v>92</v>
       </c>
       <c r="AV53" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AX53" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>58</v>
       </c>
@@ -4863,7 +4915,7 @@
         <v>38</v>
       </c>
       <c r="C54" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D54">
         <v>3.6</v>
@@ -4872,7 +4924,7 @@
         <v>68</v>
       </c>
       <c r="H54" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="S54" t="b">
         <v>0</v>
@@ -4899,19 +4951,19 @@
         <v>51</v>
       </c>
       <c r="AK54" t="s">
+        <v>165</v>
+      </c>
+      <c r="AN54">
+        <v>220</v>
+      </c>
+      <c r="AO54" t="s">
         <v>166</v>
-      </c>
-      <c r="AN54">
-        <v>220</v>
-      </c>
-      <c r="AO54" t="s">
-        <v>167</v>
       </c>
       <c r="AR54" t="s">
         <v>104</v>
       </c>
       <c r="AS54" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AU54" t="s">
         <v>104</v>
@@ -4923,7 +4975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>59</v>
       </c>
@@ -4946,7 +4998,7 @@
         <v>0</v>
       </c>
       <c r="AA55" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AB55" t="b">
         <v>1</v>
@@ -4967,28 +5019,28 @@
         <v>225</v>
       </c>
       <c r="AO55" t="s">
+        <v>169</v>
+      </c>
+      <c r="AP55" t="s">
         <v>170</v>
-      </c>
-      <c r="AP55" t="s">
-        <v>171</v>
       </c>
       <c r="AR55" t="s">
         <v>92</v>
       </c>
       <c r="AS55" t="s">
+        <v>171</v>
+      </c>
+      <c r="AU55" t="s">
         <v>172</v>
       </c>
-      <c r="AU55" t="s">
+      <c r="AV55" t="s">
         <v>173</v>
       </c>
-      <c r="AV55" t="s">
-        <v>174</v>
-      </c>
       <c r="AX55" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>60</v>
       </c>
@@ -5041,19 +5093,19 @@
         <v>5070</v>
       </c>
       <c r="AO56" t="s">
+        <v>174</v>
+      </c>
+      <c r="AS56" t="s">
         <v>175</v>
       </c>
-      <c r="AS56" t="s">
+      <c r="AV56" t="s">
         <v>176</v>
       </c>
-      <c r="AV56" t="s">
-        <v>177</v>
-      </c>
       <c r="AX56" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>61</v>
       </c>
@@ -5100,13 +5152,13 @@
         <v>52</v>
       </c>
       <c r="AP57" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AX57" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>62</v>
       </c>
@@ -5156,16 +5208,16 @@
         <v>0</v>
       </c>
       <c r="AD58" t="s">
+        <v>178</v>
+      </c>
+      <c r="AE58" t="s">
         <v>179</v>
       </c>
-      <c r="AE58" t="s">
+      <c r="AG58" t="s">
         <v>180</v>
       </c>
-      <c r="AG58" t="s">
-        <v>181</v>
-      </c>
       <c r="AH58" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AI58" t="s">
         <v>69</v>
@@ -5186,13 +5238,13 @@
         <v>111</v>
       </c>
       <c r="AP58" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AX58" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>63</v>
       </c>
@@ -5230,7 +5282,7 @@
         <v>132</v>
       </c>
       <c r="AA59" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AB59" t="b">
         <v>1</v>
@@ -5260,7 +5312,7 @@
         <v>56</v>
       </c>
       <c r="AP59" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AS59" t="s">
         <v>135</v>
@@ -5272,7 +5324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>64</v>
       </c>
@@ -5280,7 +5332,7 @@
         <v>42</v>
       </c>
       <c r="C60" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="S60" t="b">
         <v>0</v>
@@ -5301,16 +5353,16 @@
         <v>0</v>
       </c>
       <c r="AD60" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AE60" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AG60" t="s">
+        <v>160</v>
+      </c>
+      <c r="AH60" t="s">
         <v>161</v>
-      </c>
-      <c r="AH60" t="s">
-        <v>162</v>
       </c>
       <c r="AI60" t="s">
         <v>69</v>
@@ -5334,7 +5386,7 @@
         <v>56</v>
       </c>
       <c r="AP60" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AS60" t="s">
         <v>135</v>
@@ -5346,7 +5398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>65</v>
       </c>
@@ -5354,7 +5406,7 @@
         <v>43</v>
       </c>
       <c r="C61" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="S61" t="b">
         <v>0</v>
@@ -5375,16 +5427,16 @@
         <v>0</v>
       </c>
       <c r="AD61" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AE61" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AG61" t="s">
+        <v>160</v>
+      </c>
+      <c r="AH61" t="s">
         <v>161</v>
-      </c>
-      <c r="AH61" t="s">
-        <v>162</v>
       </c>
       <c r="AI61" t="s">
         <v>69</v>
@@ -5393,7 +5445,7 @@
         <v>55</v>
       </c>
       <c r="AK61" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AN61">
         <v>102</v>
@@ -5405,7 +5457,7 @@
         <v>139</v>
       </c>
       <c r="AQ61" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AR61" t="s">
         <v>72</v>
@@ -5414,7 +5466,7 @@
         <v>141</v>
       </c>
       <c r="AT61" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AU61" t="s">
         <v>74</v>
@@ -5426,7 +5478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>66</v>
       </c>
@@ -5434,7 +5486,7 @@
         <v>43</v>
       </c>
       <c r="C62" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="S62" t="b">
         <v>0</v>
@@ -5455,19 +5507,19 @@
         <v>0</v>
       </c>
       <c r="AD62" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AE62" t="s">
+        <v>188</v>
+      </c>
+      <c r="AF62" t="s">
         <v>189</v>
       </c>
-      <c r="AF62" t="s">
-        <v>190</v>
-      </c>
       <c r="AG62" t="s">
+        <v>160</v>
+      </c>
+      <c r="AH62" t="s">
         <v>161</v>
-      </c>
-      <c r="AH62" t="s">
-        <v>162</v>
       </c>
       <c r="AI62" t="s">
         <v>69</v>
@@ -5476,7 +5528,7 @@
         <v>55</v>
       </c>
       <c r="AK62" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AN62">
         <v>102</v>
@@ -5488,7 +5540,7 @@
         <v>139</v>
       </c>
       <c r="AQ62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AR62" t="s">
         <v>72</v>
@@ -5497,7 +5549,7 @@
         <v>141</v>
       </c>
       <c r="AT62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AU62" t="s">
         <v>74</v>
@@ -5509,7 +5561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>67</v>
       </c>
@@ -5556,7 +5608,7 @@
         <v>0</v>
       </c>
       <c r="AD63" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AI63" t="s">
         <v>69</v>
@@ -5580,7 +5632,7 @@
         <v>56</v>
       </c>
       <c r="AP63" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AS63" t="s">
         <v>135</v>
@@ -5592,7 +5644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>68</v>
       </c>
@@ -5648,7 +5700,7 @@
         <v>56</v>
       </c>
       <c r="AP64" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AS64" t="s">
         <v>135</v>
@@ -5660,7 +5712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>69</v>
       </c>
@@ -5725,7 +5777,7 @@
         <v>56</v>
       </c>
       <c r="AP65" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AS65" t="s">
         <v>135</v>
@@ -5737,7 +5789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>70</v>
       </c>
@@ -5745,7 +5797,7 @@
         <v>42</v>
       </c>
       <c r="C66" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D66">
         <v>14.3</v>
@@ -5805,7 +5857,7 @@
         <v>56</v>
       </c>
       <c r="AP66" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AS66" t="s">
         <v>135</v>
@@ -5817,7 +5869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>71</v>
       </c>
@@ -5876,7 +5928,7 @@
         <v>56</v>
       </c>
       <c r="AP67" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AS67" t="s">
         <v>135</v>
@@ -5888,7 +5940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>72</v>
       </c>
@@ -5941,19 +5993,19 @@
         <v>111</v>
       </c>
       <c r="AP68" t="s">
+        <v>192</v>
+      </c>
+      <c r="AS68" t="s">
         <v>193</v>
       </c>
-      <c r="AS68" t="s">
+      <c r="AV68" t="s">
         <v>194</v>
       </c>
-      <c r="AV68" t="s">
-        <v>195</v>
-      </c>
       <c r="AX68" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>74</v>
       </c>
@@ -5979,7 +6031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>75</v>
       </c>
@@ -5987,7 +6039,7 @@
         <v>48</v>
       </c>
       <c r="C70" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D70">
         <v>3.6</v>
@@ -5999,7 +6051,7 @@
         <v>2.57</v>
       </c>
       <c r="J70" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="S70" t="b">
         <v>0</v>
@@ -6020,7 +6072,7 @@
         <v>2</v>
       </c>
       <c r="AO70" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AP70" t="s">
         <v>136</v>
@@ -6032,13 +6084,13 @@
         <v>118</v>
       </c>
       <c r="AW70" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AX70" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>76</v>
       </c>
@@ -6046,7 +6098,7 @@
         <v>48</v>
       </c>
       <c r="C71" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D71">
         <v>0.38</v>
@@ -6058,7 +6110,7 @@
         <v>4.6900000000000004</v>
       </c>
       <c r="J71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="S71" t="b">
         <v>0</v>
@@ -6079,7 +6131,7 @@
         <v>2</v>
       </c>
       <c r="AO71" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AP71" t="s">
         <v>136</v>
@@ -6091,13 +6143,13 @@
         <v>118</v>
       </c>
       <c r="AW71" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AX71" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>77</v>
       </c>
@@ -6105,7 +6157,7 @@
         <v>48</v>
       </c>
       <c r="C72" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D72">
         <v>1.27</v>
@@ -6117,7 +6169,7 @@
         <v>2.29</v>
       </c>
       <c r="J72" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="S72" t="b">
         <v>0</v>
@@ -6138,7 +6190,7 @@
         <v>2</v>
       </c>
       <c r="AO72" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AP72" t="s">
         <v>136</v>
@@ -6150,13 +6202,13 @@
         <v>118</v>
       </c>
       <c r="AW72" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AX72" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:50" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:50" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>78</v>
       </c>
@@ -6176,7 +6228,7 @@
         <v>106</v>
       </c>
       <c r="J73" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K73" s="1">
         <v>1</v>
@@ -6194,19 +6246,19 @@
         <v>4295</v>
       </c>
       <c r="P73" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Q73" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="S73" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="T73" s="1" t="b">
         <v>0</v>
       </c>
       <c r="V73" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="W73" s="1" t="b">
         <v>0</v>
@@ -6218,10 +6270,10 @@
         <v>94</v>
       </c>
       <c r="Z73" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="AA73" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="AA73" s="2" t="s">
-        <v>222</v>
       </c>
       <c r="AB73" s="1" t="b">
         <v>1</v>
@@ -6230,19 +6282,19 @@
         <v>0</v>
       </c>
       <c r="AD73" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AE73" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AF73" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AG73" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AH73" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AI73" s="2" t="s">
         <v>69</v>
@@ -6260,34 +6312,34 @@
         <v>97</v>
       </c>
       <c r="AP73" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AQ73" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AR73" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AS73" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AT73" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AU73" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AV73" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AW73" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AX73" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>79</v>
       </c>
@@ -6331,7 +6383,7 @@
         <v>94</v>
       </c>
       <c r="AA74" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AB74" t="b">
         <v>1</v>
@@ -6355,28 +6407,28 @@
         <v>225</v>
       </c>
       <c r="AO74" t="s">
+        <v>169</v>
+      </c>
+      <c r="AP74" t="s">
         <v>170</v>
-      </c>
-      <c r="AP74" t="s">
-        <v>171</v>
       </c>
       <c r="AR74" t="s">
         <v>92</v>
       </c>
       <c r="AS74" t="s">
+        <v>171</v>
+      </c>
+      <c r="AU74" t="s">
         <v>172</v>
       </c>
-      <c r="AU74" t="s">
+      <c r="AV74" t="s">
         <v>173</v>
       </c>
-      <c r="AV74" t="s">
-        <v>174</v>
-      </c>
       <c r="AX74" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>80</v>
       </c>
@@ -6426,7 +6478,7 @@
         <v>56</v>
       </c>
       <c r="AP75" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AT75" t="s">
         <v>91</v>
@@ -6441,7 +6493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>81</v>
       </c>
@@ -6449,7 +6501,7 @@
         <v>51</v>
       </c>
       <c r="C76" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D76">
         <v>3.6000000000000002E-4</v>
@@ -6464,7 +6516,7 @@
         <v>2.5700000000000001E-4</v>
       </c>
       <c r="J76" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="S76" t="b">
         <v>0</v>
@@ -6482,13 +6534,13 @@
         <v>0</v>
       </c>
       <c r="AW76" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AX76" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>82</v>
       </c>
@@ -6496,7 +6548,7 @@
         <v>51</v>
       </c>
       <c r="C77" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D77">
         <v>3.8000000000000002E-5</v>
@@ -6511,7 +6563,7 @@
         <v>4.6900000000000002E-4</v>
       </c>
       <c r="J77" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="S77" t="b">
         <v>0</v>
@@ -6529,13 +6581,13 @@
         <v>0</v>
       </c>
       <c r="AW77" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AX77" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>83</v>
       </c>
@@ -6543,7 +6595,7 @@
         <v>51</v>
       </c>
       <c r="C78" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D78">
         <v>1.27E-4</v>
@@ -6558,7 +6610,7 @@
         <v>2.2900000000000001E-4</v>
       </c>
       <c r="J78" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="S78" t="b">
         <v>0</v>
@@ -6576,13 +6628,13 @@
         <v>0</v>
       </c>
       <c r="AW78" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AX78" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>84</v>
       </c>
@@ -6623,7 +6675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>86</v>
       </c>
@@ -6676,13 +6728,13 @@
         <v>65</v>
       </c>
       <c r="AP80" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AX80" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>87</v>
       </c>
@@ -6714,7 +6766,7 @@
         <v>0</v>
       </c>
       <c r="X81" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AB81" t="b">
         <v>0</v>
@@ -6732,13 +6784,13 @@
         <v>675</v>
       </c>
       <c r="AO81" t="s">
+        <v>207</v>
+      </c>
+      <c r="AP81" t="s">
         <v>208</v>
       </c>
-      <c r="AP81" t="s">
+      <c r="AS81" t="s">
         <v>209</v>
-      </c>
-      <c r="AS81" t="s">
-        <v>210</v>
       </c>
       <c r="AV81" t="s">
         <v>105</v>
@@ -6747,7 +6799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>88</v>
       </c>
@@ -6806,19 +6858,19 @@
         <v>111</v>
       </c>
       <c r="AP82" t="s">
+        <v>210</v>
+      </c>
+      <c r="AS82" t="s">
         <v>211</v>
       </c>
-      <c r="AS82" t="s">
+      <c r="AV82" t="s">
         <v>212</v>
       </c>
-      <c r="AV82" t="s">
-        <v>213</v>
-      </c>
       <c r="AX82" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>89</v>
       </c>
@@ -6880,19 +6932,19 @@
         <v>111</v>
       </c>
       <c r="AP83" t="s">
+        <v>210</v>
+      </c>
+      <c r="AS83" t="s">
         <v>211</v>
       </c>
-      <c r="AS83" t="s">
+      <c r="AV83" t="s">
         <v>212</v>
       </c>
-      <c r="AV83" t="s">
-        <v>213</v>
-      </c>
       <c r="AX83" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>90</v>
       </c>
@@ -6954,25 +7006,25 @@
         <v>111</v>
       </c>
       <c r="AP84" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AR84" t="s">
         <v>125</v>
       </c>
       <c r="AS84" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AU84" t="s">
         <v>125</v>
       </c>
       <c r="AV84" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AX84" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>92</v>
       </c>
@@ -6980,7 +7032,7 @@
         <v>58</v>
       </c>
       <c r="C85" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="S85" t="b">
         <v>0</v>
@@ -6998,16 +7050,16 @@
         <v>0</v>
       </c>
       <c r="AD85" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AE85" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AF85" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AG85" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AH85" t="s">
         <v>100</v>
@@ -7031,25 +7083,25 @@
         <v>111</v>
       </c>
       <c r="AP85" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AR85" t="s">
         <v>125</v>
       </c>
       <c r="AS85" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AU85" t="s">
         <v>125</v>
       </c>
       <c r="AV85" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AX85" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>94</v>
       </c>
@@ -7057,7 +7109,7 @@
         <v>58</v>
       </c>
       <c r="C86" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="S86" t="b">
         <v>0</v>
@@ -7075,13 +7127,13 @@
         <v>0</v>
       </c>
       <c r="AD86" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AE86" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AG86" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AH86" t="s">
         <v>100</v>
@@ -7108,19 +7160,19 @@
         <v>125</v>
       </c>
       <c r="AS86" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AU86" t="s">
         <v>125</v>
       </c>
       <c r="AV86" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AX86" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>100</v>
       </c>
@@ -7128,7 +7180,7 @@
         <v>42</v>
       </c>
       <c r="C87" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="S87" t="b">
         <v>0</v>
@@ -7149,16 +7201,16 @@
         <v>0</v>
       </c>
       <c r="AD87" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AE87" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AG87" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AH87" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AI87" t="s">
         <v>69</v>
@@ -7182,7 +7234,7 @@
         <v>56</v>
       </c>
       <c r="AP87" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AS87" t="s">
         <v>135</v>
@@ -7194,7 +7246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>101</v>
       </c>
@@ -7202,7 +7254,7 @@
         <v>63</v>
       </c>
       <c r="C88" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D88">
         <v>0.3</v>
@@ -7229,7 +7281,7 @@
         <v>51</v>
       </c>
       <c r="Y88" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AA88" t="s">
         <v>121</v>
@@ -7250,28 +7302,28 @@
         <v>308</v>
       </c>
       <c r="AO88" t="s">
+        <v>216</v>
+      </c>
+      <c r="AP88" t="s">
         <v>217</v>
       </c>
-      <c r="AP88" t="s">
+      <c r="AR88" t="s">
         <v>218</v>
       </c>
-      <c r="AR88" t="s">
+      <c r="AS88" t="s">
         <v>219</v>
-      </c>
-      <c r="AS88" t="s">
-        <v>220</v>
       </c>
       <c r="AU88" t="s">
         <v>92</v>
       </c>
       <c r="AV88" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AX88" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:50" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:50" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="5">
         <v>102</v>
       </c>
@@ -7321,7 +7373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:50" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:50" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="5">
         <v>103</v>
       </c>
@@ -7365,7 +7417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:50" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:50" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="5">
         <v>104</v>
       </c>
@@ -7421,7 +7473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:50" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:50" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="5">
         <v>105</v>
       </c>
@@ -7471,7 +7523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>106</v>
       </c>
@@ -7521,7 +7573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:50" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:50" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="5">
         <v>107</v>
       </c>
@@ -7565,7 +7617,7 @@
         <v>94</v>
       </c>
       <c r="AA94" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AB94" s="5" t="b">
         <v>1</v>
@@ -7589,7 +7641,7 @@
         <v>97</v>
       </c>
       <c r="AP94" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AX94" s="5" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
addional parameter context for param id 54
</commit_message>
<xml_diff>
--- a/data/marburg/raw/marburg_parameter_new.xlsx
+++ b/data/marburg/raw/marburg_parameter_new.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cm401/priority_pathogen_review/data/marburg/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091C5CDF-D673-CB48-B6DE-13BB63956312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC9E6A0-8526-7B41-BB8C-8149A7D5A38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter_data___Table" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Parameter_data___Table!$A$1:$AX$94</definedName>
     <definedName name="Parameter_data___Table">Parameter_data___Table!$A$1:$AX$88</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="223">
   <si>
     <t>Parameter_data_ID</t>
   </si>
@@ -689,6 +690,9 @@
   </si>
   <si>
     <t>Age, Region, Sex</t>
+  </si>
+  <si>
+    <t>Python cave, Kitake mine</t>
   </si>
 </sst>
 </file>
@@ -1105,9 +1109,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AP52" sqref="AP52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1369,7 +1373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:50" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:50" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1488,7 +1492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:50" ht="64" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:50" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1607,7 +1611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:50" ht="64" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:50" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1727,7 +1731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:50" ht="64" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:50" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -1846,7 +1850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:50" ht="64" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:50" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -4785,6 +4789,12 @@
       <c r="AH51" t="s">
         <v>161</v>
       </c>
+      <c r="AO51" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP51" t="s">
+        <v>222</v>
+      </c>
       <c r="AX51" t="b">
         <v>0</v>
       </c>
@@ -7648,6 +7658,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AX94" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update to riskfactor_outcome on re-run of raw data
</commit_message>
<xml_diff>
--- a/data/marburg/raw/marburg_parameter_new.xlsx
+++ b/data/marburg/raw/marburg_parameter_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cm401/priority_pathogen_review/data/marburg/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC9E6A0-8526-7B41-BB8C-8149A7D5A38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C52E25-1683-1941-9664-65DD9BCECF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter_data___Table" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="223">
   <si>
     <t>Parameter_data_ID</t>
   </si>
@@ -1109,9 +1109,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AP52" sqref="AP52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AD39" sqref="AD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2401,6 +2401,9 @@
       <c r="AC15" t="b">
         <v>0</v>
       </c>
+      <c r="AD15" t="s">
+        <v>51</v>
+      </c>
       <c r="AI15" t="s">
         <v>78</v>
       </c>
@@ -3940,6 +3943,9 @@
       <c r="AC39" t="b">
         <v>0</v>
       </c>
+      <c r="AD39" t="s">
+        <v>190</v>
+      </c>
       <c r="AI39" t="s">
         <v>69</v>
       </c>
@@ -4167,6 +4173,9 @@
       </c>
       <c r="AC42" t="b">
         <v>0</v>
+      </c>
+      <c r="AD42" t="s">
+        <v>190</v>
       </c>
       <c r="AI42" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
updates to data; add in cleaning of dates for outbreaks
</commit_message>
<xml_diff>
--- a/data/marburg/raw/marburg_parameter_new.xlsx
+++ b/data/marburg/raw/marburg_parameter_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cm401/priority_pathogen_review/data/marburg/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/kem22_ic_ac_uk/Documents/Projects/Priority Pathogens/priority-pathogens/data/marburg/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C52E25-1683-1941-9664-65DD9BCECF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{F8C52E25-1683-1941-9664-65DD9BCECF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4FBA9B4-821F-46DE-8D81-44F5FE3A25D8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter_data___Table" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="223">
   <si>
     <t>Parameter_data_ID</t>
   </si>
@@ -787,9 +787,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -827,9 +827,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -862,26 +862,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -914,26 +897,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1109,66 +1075,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AD39" sqref="AD39"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V28" sqref="V28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="14" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="22" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="16" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="17" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="94.1640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="86.83203125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="94.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="86.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="11" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1320,7 +1286,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1373,7 +1339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:50" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1407,22 +1373,16 @@
       <c r="Q3" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="S3" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="T3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>220</v>
+      <c r="S3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="V3" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="W3" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="X3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>58</v>
       </c>
       <c r="Z3" s="2" t="s">
@@ -1492,7 +1452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:50" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1526,22 +1486,16 @@
       <c r="Q4" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="S4" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="T4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>220</v>
+      <c r="S4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="V4" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="W4" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="X4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="2" t="s">
+      <c r="X4" s="2" t="s">
         <v>58</v>
       </c>
       <c r="Z4" s="2" t="s">
@@ -1611,7 +1565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:50" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1646,22 +1600,16 @@
       <c r="Q5" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="S5" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="T5" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>220</v>
+      <c r="S5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="V5" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="W5" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="X5" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="2" t="s">
+      <c r="X5" s="2" t="s">
         <v>58</v>
       </c>
       <c r="Z5" s="2" t="s">
@@ -1731,7 +1679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:50" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:50" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -1765,22 +1713,16 @@
       <c r="Q6" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="S6" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="T6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="V6" s="2" t="s">
-        <v>220</v>
+      <c r="S6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="V6" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="W6" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="X6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="2" t="s">
+      <c r="X6" s="2" t="s">
         <v>58</v>
       </c>
       <c r="Z6" s="2" t="s">
@@ -1850,7 +1792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:50" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:50" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -1884,22 +1826,16 @@
       <c r="Q7" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="S7" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="T7" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="V7" s="2" t="s">
-        <v>220</v>
+      <c r="S7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="V7" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="W7" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="X7" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="2" t="s">
+      <c r="X7" s="2" t="s">
         <v>58</v>
       </c>
       <c r="Z7" s="2" t="s">
@@ -1969,7 +1905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -2019,7 +1955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -2075,7 +2011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>11</v>
       </c>
@@ -2137,7 +2073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>12</v>
       </c>
@@ -2202,7 +2138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>13</v>
       </c>
@@ -2252,7 +2188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>14</v>
       </c>
@@ -2317,7 +2253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>15</v>
       </c>
@@ -2367,7 +2303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>16</v>
       </c>
@@ -2432,7 +2368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>17</v>
       </c>
@@ -2497,7 +2433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>18</v>
       </c>
@@ -2550,7 +2486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>19</v>
       </c>
@@ -2636,7 +2572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20</v>
       </c>
@@ -2695,7 +2631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>21</v>
       </c>
@@ -2766,7 +2702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>22</v>
       </c>
@@ -2828,7 +2764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>23</v>
       </c>
@@ -2887,7 +2823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>24</v>
       </c>
@@ -2955,7 +2891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>25</v>
       </c>
@@ -3026,7 +2962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>26</v>
       </c>
@@ -3100,7 +3036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>27</v>
       </c>
@@ -3156,7 +3092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>29</v>
       </c>
@@ -3206,7 +3142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>30</v>
       </c>
@@ -3262,7 +3198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>31</v>
       </c>
@@ -3288,7 +3224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>32</v>
       </c>
@@ -3359,7 +3295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>33</v>
       </c>
@@ -3421,7 +3357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>34</v>
       </c>
@@ -3471,7 +3407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>35</v>
       </c>
@@ -3530,7 +3466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>36</v>
       </c>
@@ -3598,7 +3534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>37</v>
       </c>
@@ -3678,7 +3614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>38</v>
       </c>
@@ -3725,7 +3661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>40</v>
       </c>
@@ -3811,7 +3747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>41</v>
       </c>
@@ -3897,7 +3833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>42</v>
       </c>
@@ -3986,7 +3922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>43</v>
       </c>
@@ -4042,7 +3978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>44</v>
       </c>
@@ -4128,7 +4064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>45</v>
       </c>
@@ -4217,7 +4153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>46</v>
       </c>
@@ -4303,7 +4239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>47</v>
       </c>
@@ -4356,7 +4292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>48</v>
       </c>
@@ -4442,7 +4378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>49</v>
       </c>
@@ -4483,7 +4419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>50</v>
       </c>
@@ -4530,7 +4466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>51</v>
       </c>
@@ -4577,7 +4513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>52</v>
       </c>
@@ -4666,7 +4602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>53</v>
       </c>
@@ -4761,7 +4697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>54</v>
       </c>
@@ -4808,7 +4744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>55</v>
       </c>
@@ -4855,7 +4791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>57</v>
       </c>
@@ -4926,7 +4862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>58</v>
       </c>
@@ -4994,7 +4930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>59</v>
       </c>
@@ -5059,7 +4995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>60</v>
       </c>
@@ -5124,7 +5060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>61</v>
       </c>
@@ -5177,7 +5113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>62</v>
       </c>
@@ -5263,7 +5199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>63</v>
       </c>
@@ -5343,7 +5279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>64</v>
       </c>
@@ -5417,7 +5353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>65</v>
       </c>
@@ -5497,7 +5433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>66</v>
       </c>
@@ -5580,7 +5516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>67</v>
       </c>
@@ -5663,7 +5599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>68</v>
       </c>
@@ -5731,7 +5667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>69</v>
       </c>
@@ -5808,7 +5744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>70</v>
       </c>
@@ -5888,7 +5824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>71</v>
       </c>
@@ -5959,7 +5895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>72</v>
       </c>
@@ -6024,7 +5960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>74</v>
       </c>
@@ -6050,7 +5986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>75</v>
       </c>
@@ -6109,7 +6045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>76</v>
       </c>
@@ -6168,7 +6104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>77</v>
       </c>
@@ -6227,7 +6163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:50" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:50" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>78</v>
       </c>
@@ -6270,22 +6206,19 @@
       <c r="Q73" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="S73" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="T73" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="V73" s="2" t="s">
-        <v>220</v>
+      <c r="S73" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="U73" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="V73" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="W73" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="X73" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y73" s="2" t="s">
+      <c r="X73" s="2" t="s">
         <v>94</v>
       </c>
       <c r="Z73" s="2" t="s">
@@ -6358,7 +6291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>79</v>
       </c>
@@ -6447,7 +6380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>80</v>
       </c>
@@ -6512,7 +6445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>81</v>
       </c>
@@ -6559,7 +6492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>82</v>
       </c>
@@ -6606,7 +6539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>83</v>
       </c>
@@ -6653,7 +6586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>84</v>
       </c>
@@ -6694,7 +6627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>86</v>
       </c>
@@ -6753,7 +6686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>87</v>
       </c>
@@ -6818,7 +6751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>88</v>
       </c>
@@ -6889,7 +6822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>89</v>
       </c>
@@ -6963,7 +6896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>90</v>
       </c>
@@ -7043,7 +6976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>92</v>
       </c>
@@ -7120,7 +7053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>94</v>
       </c>
@@ -7191,7 +7124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>100</v>
       </c>
@@ -7265,7 +7198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>101</v>
       </c>
@@ -7342,7 +7275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:50" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:50" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>102</v>
       </c>
@@ -7392,7 +7325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:50" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:50" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>103</v>
       </c>
@@ -7436,7 +7369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:50" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:50" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
         <v>104</v>
       </c>
@@ -7492,7 +7425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:50" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:50" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>105</v>
       </c>
@@ -7542,7 +7475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>106</v>
       </c>
@@ -7592,7 +7525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:50" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:50" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>107</v>
       </c>
@@ -7667,7 +7600,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AX94" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AX94" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AX94">
+      <sortCondition ref="A1:A94"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>